<commit_message>
Filled out all I can
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billy\OneDrive\Desktop\Software Technologies\GitWorkspace\Project Management\2810ICT-Project-Management-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FB64A7-1B87-4992-BB18-A3B24FFDEA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8DCF84-4690-496A-8FDE-2A80F95B15E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,87 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>PERIODS</t>
-  </si>
-  <si>
-    <t>Activity 01</t>
-  </si>
-  <si>
-    <t>Activity 02</t>
-  </si>
-  <si>
-    <t>Activity 03</t>
-  </si>
-  <si>
-    <t>Activity 04</t>
-  </si>
-  <si>
-    <t>Activity 05</t>
-  </si>
-  <si>
-    <t>Activity 06</t>
-  </si>
-  <si>
-    <t>Activity 07</t>
-  </si>
-  <si>
-    <t>Activity 08</t>
-  </si>
-  <si>
-    <t>Activity 09</t>
-  </si>
-  <si>
-    <t>Activity 10</t>
-  </si>
-  <si>
-    <t>Activity 11</t>
-  </si>
-  <si>
-    <t>Activity 12</t>
-  </si>
-  <si>
-    <t>Activity 13</t>
-  </si>
-  <si>
-    <t>Activity 14</t>
-  </si>
-  <si>
-    <t>Activity 15</t>
-  </si>
-  <si>
-    <t>Activity 16</t>
-  </si>
-  <si>
-    <t>Activity 17</t>
-  </si>
-  <si>
-    <t>Activity 18</t>
-  </si>
-  <si>
-    <t>Activity 19</t>
-  </si>
-  <si>
-    <t>Activity 20</t>
-  </si>
-  <si>
-    <t>Activity 21</t>
-  </si>
-  <si>
-    <t>Activity 22</t>
-  </si>
-  <si>
-    <t>Activity 23</t>
-  </si>
-  <si>
-    <t>Activity 24</t>
-  </si>
-  <si>
-    <t>Activity 25</t>
-  </si>
-  <si>
-    <t>Activity 26</t>
   </si>
   <si>
     <r>
@@ -207,33 +129,6 @@
     <t>Plan Duration</t>
   </si>
   <si>
-    <t>Activity 27</t>
-  </si>
-  <si>
-    <t>Activity 28</t>
-  </si>
-  <si>
-    <t>Activity 29</t>
-  </si>
-  <si>
-    <t>Activity 30</t>
-  </si>
-  <si>
-    <t>Activity 31</t>
-  </si>
-  <si>
-    <t>Activity 32</t>
-  </si>
-  <si>
-    <t>Activity 33</t>
-  </si>
-  <si>
-    <t>Activity 34</t>
-  </si>
-  <si>
-    <t>Activity 35</t>
-  </si>
-  <si>
     <t>Plan
 Start</t>
   </si>
@@ -262,13 +157,106 @@
   </si>
   <si>
     <t>Comprehensive Food GUI</t>
+  </si>
+  <si>
+    <t>1.1 Define Project Objectives</t>
+  </si>
+  <si>
+    <t>1.2 Identify Project Stakeholders</t>
+  </si>
+  <si>
+    <t>2.1 Define Project Scope</t>
+  </si>
+  <si>
+    <t>2.2 Create WBS</t>
+  </si>
+  <si>
+    <t>2.3.1 Define and Sequence Activities</t>
+  </si>
+  <si>
+    <t>2.3.2 Estimate Activity Duration</t>
+  </si>
+  <si>
+    <t>2.4.1 Define Problem Background</t>
+  </si>
+  <si>
+    <t>2.4.2 Define System Capabilities / Overview</t>
+  </si>
+  <si>
+    <t>2.4.3 Identify the Benefits</t>
+  </si>
+  <si>
+    <t>2.5.1 Identify User Requirements</t>
+  </si>
+  <si>
+    <t>2.5.2 Identify Software Requirements</t>
+  </si>
+  <si>
+    <t>2.5.3 Identify Use Cases and Consruct Diagrams</t>
+  </si>
+  <si>
+    <t>2.6.1 Design Software</t>
+  </si>
+  <si>
+    <t>2.6.2 Identify System Components</t>
+  </si>
+  <si>
+    <t>2.7.1 Design the Structure</t>
+  </si>
+  <si>
+    <t>2.7.2 Design the Visuals</t>
+  </si>
+  <si>
+    <t>3.1 Implement the GUI</t>
+  </si>
+  <si>
+    <t>3.2 Implement the Food Search Feature</t>
+  </si>
+  <si>
+    <t>3.3 Implement Nutrition Breakdown Feature</t>
+  </si>
+  <si>
+    <t>3.4 Implement Nutrition Range Filter Feature</t>
+  </si>
+  <si>
+    <t>3.5 Implement Nutrition Level Filter Feature</t>
+  </si>
+  <si>
+    <t>3.6 Implement ADDITIONAL FEATURE</t>
+  </si>
+  <si>
+    <t>3.7 Conduct Testing</t>
+  </si>
+  <si>
+    <t>4.1 Track Progress</t>
+  </si>
+  <si>
+    <t>4.2 Control Scope</t>
+  </si>
+  <si>
+    <t>4.3 Control Quality</t>
+  </si>
+  <si>
+    <t>4.4 Monitor Bugs</t>
+  </si>
+  <si>
+    <t>5.1 Review and Complete Work</t>
+  </si>
+  <si>
+    <t>5.2 Performance Review</t>
+  </si>
+  <si>
+    <t>5.3 Verify Completion of Work</t>
+  </si>
+  <si>
+    <t>Ongoing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -373,7 +361,13 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="1" tint="0.24994659260841701"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1" tint="0.24994659260841701"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -565,7 +559,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -635,9 +629,6 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -676,6 +667,12 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1077,10 +1074,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO39"/>
+  <dimension ref="B1:BM40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="94" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1096,9 +1093,9 @@
     <col min="42" max="42" width="2.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
+    <row r="1" spans="2:65" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
       <c r="B1" s="11" t="s">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -1106,53 +1103,53 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:67" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
+    <row r="2" spans="2:65" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2" s="21" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="H2" s="12">
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="L2" s="27"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="27"/>
-      <c r="O2" s="28"/>
+      <c r="K2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="27"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="26" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="28"/>
+      <c r="Q2" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="27"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="W2" s="31"/>
-      <c r="X2" s="31"/>
-      <c r="Y2" s="32"/>
+      <c r="V2" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="30"/>
+      <c r="X2" s="30"/>
+      <c r="Y2" s="31"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="AB2" s="31"/>
-      <c r="AC2" s="31"/>
-      <c r="AD2" s="31"/>
-      <c r="AE2" s="31"/>
-      <c r="AF2" s="31"/>
-      <c r="AG2" s="32"/>
+      <c r="AA2" s="29" t="s">
+        <v>2</v>
+      </c>
+      <c r="AB2" s="30"/>
+      <c r="AC2" s="30"/>
+      <c r="AD2" s="30"/>
+      <c r="AE2" s="30"/>
+      <c r="AF2" s="30"/>
+      <c r="AG2" s="31"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="AJ2" s="20"/>
       <c r="AK2" s="20"/>
@@ -1162,24 +1159,24 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:67" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="34" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>45</v>
+    <row r="3" spans="2:65" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="35" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
         <v>0</v>
@@ -1204,13 +1201,13 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="35"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
+    <row r="4" spans="2:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="34"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1385,163 +1382,229 @@
       <c r="BM4" s="3">
         <v>58</v>
       </c>
-      <c r="BN4" s="3">
-        <v>59</v>
-      </c>
-      <c r="BO4" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="23" t="s">
-        <v>1</v>
+    </row>
+    <row r="5" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B5" s="36" t="s">
+        <v>14</v>
       </c>
       <c r="C5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="5">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F5" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G5" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B6" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
       <c r="D6" s="5">
-        <v>0</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="E6" s="5">
+        <v>9</v>
+      </c>
+      <c r="F6" s="5">
+        <v>18</v>
+      </c>
       <c r="G6" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B7" s="36" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="5">
+        <v>4</v>
+      </c>
+      <c r="D7" s="5">
         <v>3</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="5">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5">
+        <v>9</v>
+      </c>
       <c r="G7" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B8" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="5">
+        <v>7</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5">
+        <v>31</v>
+      </c>
+      <c r="F8" s="5">
+        <v>1</v>
+      </c>
       <c r="G8" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B9" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="5">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>31</v>
+      </c>
+      <c r="F9" s="5">
+        <v>1</v>
+      </c>
       <c r="G9" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B10" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="5">
+        <v>11</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5">
+        <v>31</v>
+      </c>
+      <c r="F10" s="5">
+        <v>1</v>
+      </c>
       <c r="G10" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B11" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="5">
+        <v>12</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>29</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1</v>
+      </c>
       <c r="G11" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B12" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="5">
+        <v>13</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2</v>
+      </c>
+      <c r="E12" s="5">
+        <v>29</v>
+      </c>
+      <c r="F12" s="5">
+        <v>1</v>
+      </c>
       <c r="G12" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B13" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="5">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
+        <v>29</v>
+      </c>
+      <c r="F13" s="5">
+        <v>2</v>
+      </c>
       <c r="G13" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B14" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="5">
+        <v>16</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
+    <row r="15" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B15" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="6">
+        <v>17</v>
+      </c>
+      <c r="D15" s="5">
+        <v>2</v>
+      </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+    <row r="16" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B16" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="5">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="22">
@@ -1549,11 +1612,15 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="B17" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="5">
+        <v>21</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="22">
@@ -1561,23 +1628,33 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
+      <c r="B18" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="5">
+        <v>23</v>
+      </c>
+      <c r="D18" s="5">
+        <v>3</v>
+      </c>
+      <c r="E18" s="5">
+        <v>30</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="22">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="B19" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="5">
+        <v>26</v>
+      </c>
+      <c r="D19" s="5">
+        <v>2</v>
+      </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="22">
@@ -1585,11 +1662,15 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="B20" s="36" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="5">
+        <v>28</v>
+      </c>
+      <c r="D20" s="5">
+        <v>2</v>
+      </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="22">
@@ -1597,11 +1678,15 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="5">
+        <v>30</v>
+      </c>
+      <c r="D21" s="5">
+        <v>3</v>
+      </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="22">
@@ -1609,11 +1694,15 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="23" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="5">
+        <v>33</v>
+      </c>
+      <c r="D22" s="5">
+        <v>3</v>
+      </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="22">
@@ -1621,11 +1710,15 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="5">
+        <v>36</v>
+      </c>
+      <c r="D23" s="5">
+        <v>3</v>
+      </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="22">
@@ -1633,11 +1726,15 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
+      <c r="B24" s="36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="5">
+        <v>39</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3</v>
+      </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
       <c r="G24" s="22">
@@ -1645,11 +1742,15 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C25" s="5">
+        <v>42</v>
+      </c>
+      <c r="D25" s="5">
+        <v>3</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="22">
@@ -1657,11 +1758,15 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B26" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="B26" s="36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="5">
+        <v>45</v>
+      </c>
+      <c r="D26" s="5">
+        <v>3</v>
+      </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
       <c r="G26" s="22">
@@ -1669,11 +1774,15 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="B27" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="5">
+        <v>50</v>
+      </c>
+      <c r="D27" s="5">
+        <v>5</v>
+      </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="22">
@@ -1681,11 +1790,15 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B28" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="B28" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="5">
+        <v>1</v>
+      </c>
+      <c r="D28" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
       <c r="G28" s="22">
@@ -1693,11 +1806,15 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="B29" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="5">
+        <v>30</v>
+      </c>
+      <c r="D29" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="22">
@@ -1705,11 +1822,15 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="B30" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="5">
+        <v>30</v>
+      </c>
+      <c r="D30" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="22">
@@ -1717,11 +1838,15 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="B31" s="36" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" s="5">
+        <v>30</v>
+      </c>
+      <c r="D31" s="37" t="s">
+        <v>44</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="22">
@@ -1729,100 +1854,220 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="B32" s="36" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" s="5">
+        <v>55</v>
+      </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="23" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+    <row r="33" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B33" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" s="5">
+        <v>56</v>
+      </c>
+      <c r="D33" s="5">
+        <v>1</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B34" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+    <row r="34" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B34" s="36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="5">
+        <v>57</v>
+      </c>
+      <c r="D34" s="5">
+        <v>1</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="22">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B35" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B36" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B37" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B38" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B39" s="23" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="22">
-        <v>0</v>
-      </c>
+    <row r="35" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+    </row>
+    <row r="36" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+    </row>
+    <row r="37" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+    </row>
+    <row r="38" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+      <c r="Z38"/>
+      <c r="AA38"/>
+    </row>
+    <row r="39" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+      <c r="Z39"/>
+      <c r="AA39"/>
+    </row>
+    <row r="40" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40"/>
+      <c r="AA40"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1838,12 +2083,12 @@
     <mergeCell ref="V2:Y2"/>
     <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:BO4">
+  <conditionalFormatting sqref="H4:BM4">
     <cfRule type="expression" dxfId="8" priority="8">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BO39">
+  <conditionalFormatting sqref="H5:BM34">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
changes to gantt chart apparently
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billy\OneDrive\Desktop\Software Technologies\GitWorkspace\Project Management\2810ICT-Project-Management-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8DCF84-4690-496A-8FDE-2A80F95B15E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A03599-98DA-4C76-8E48-5CE89D857CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -629,12 +629,30 @@
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -655,24 +673,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1076,8 +1076,8 @@
   </sheetPr>
   <dimension ref="B1:BM40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="94" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="BQ2" sqref="BQ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1104,11 +1104,11 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:65" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1116,37 +1116,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="25" t="s">
+      <c r="K2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="27"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="25" t="s">
+      <c r="Q2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="28"/>
-      <c r="S2" s="28"/>
-      <c r="T2" s="27"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="30"/>
-      <c r="X2" s="30"/>
-      <c r="Y2" s="31"/>
+      <c r="V2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="29" t="s">
+      <c r="AA2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="30"/>
-      <c r="AC2" s="30"/>
-      <c r="AD2" s="30"/>
-      <c r="AE2" s="30"/>
-      <c r="AF2" s="30"/>
-      <c r="AG2" s="31"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="37"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1160,22 +1160,22 @@
       <c r="AP2" s="20"/>
     </row>
     <row r="3" spans="2:65" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="35" t="s">
+      <c r="D3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="35" t="s">
+      <c r="F3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="30" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1202,12 +1202,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="34"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1384,7 +1384,7 @@
       </c>
     </row>
     <row r="5" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="23" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="5">
@@ -1404,7 +1404,7 @@
       </c>
     </row>
     <row r="6" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B6" s="36" t="s">
+      <c r="B6" s="23" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="5">
@@ -1424,7 +1424,7 @@
       </c>
     </row>
     <row r="7" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="23" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="5">
@@ -1444,7 +1444,7 @@
       </c>
     </row>
     <row r="8" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="23" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="5">
@@ -1464,7 +1464,7 @@
       </c>
     </row>
     <row r="9" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="5">
@@ -1484,7 +1484,7 @@
       </c>
     </row>
     <row r="10" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="23" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="5">
@@ -1504,7 +1504,7 @@
       </c>
     </row>
     <row r="11" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="23" t="s">
         <v>20</v>
       </c>
       <c r="C11" s="5">
@@ -1524,7 +1524,7 @@
       </c>
     </row>
     <row r="12" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C12" s="5">
@@ -1544,7 +1544,7 @@
       </c>
     </row>
     <row r="13" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="5">
@@ -1564,7 +1564,7 @@
       </c>
     </row>
     <row r="14" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B14" s="36" t="s">
+      <c r="B14" s="23" t="s">
         <v>23</v>
       </c>
       <c r="C14" s="5">
@@ -1580,7 +1580,7 @@
       </c>
     </row>
     <row r="15" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B15" s="36" t="s">
+      <c r="B15" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C15" s="6">
@@ -1596,7 +1596,7 @@
       </c>
     </row>
     <row r="16" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B16" s="36" t="s">
+      <c r="B16" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C16" s="5">
@@ -1612,7 +1612,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B17" s="36" t="s">
+      <c r="B17" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="5">
@@ -1628,7 +1628,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B18" s="36" t="s">
+      <c r="B18" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="5">
@@ -1646,7 +1646,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B19" s="36" t="s">
+      <c r="B19" s="23" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="5">
@@ -1662,7 +1662,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B20" s="36" t="s">
+      <c r="B20" s="23" t="s">
         <v>29</v>
       </c>
       <c r="C20" s="5">
@@ -1678,7 +1678,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C21" s="5">
@@ -1694,7 +1694,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B22" s="36" t="s">
+      <c r="B22" s="23" t="s">
         <v>31</v>
       </c>
       <c r="C22" s="5">
@@ -1710,7 +1710,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B23" s="36" t="s">
+      <c r="B23" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="5">
@@ -1726,7 +1726,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="23" t="s">
         <v>33</v>
       </c>
       <c r="C24" s="5">
@@ -1742,7 +1742,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B25" s="36" t="s">
+      <c r="B25" s="23" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="5">
@@ -1758,7 +1758,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B26" s="36" t="s">
+      <c r="B26" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="5">
@@ -1774,7 +1774,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B27" s="36" t="s">
+      <c r="B27" s="23" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="5">
@@ -1790,13 +1790,13 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="23" t="s">
         <v>37</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
       </c>
-      <c r="D28" s="37" t="s">
+      <c r="D28" s="24" t="s">
         <v>44</v>
       </c>
       <c r="E28" s="5"/>
@@ -1806,13 +1806,13 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="23" t="s">
         <v>38</v>
       </c>
       <c r="C29" s="5">
         <v>30</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="24" t="s">
         <v>44</v>
       </c>
       <c r="E29" s="5"/>
@@ -1822,13 +1822,13 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B30" s="36" t="s">
+      <c r="B30" s="23" t="s">
         <v>39</v>
       </c>
       <c r="C30" s="5">
         <v>30</v>
       </c>
-      <c r="D30" s="37" t="s">
+      <c r="D30" s="24" t="s">
         <v>44</v>
       </c>
       <c r="E30" s="5"/>
@@ -1838,13 +1838,13 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="23" t="s">
         <v>40</v>
       </c>
       <c r="C31" s="5">
         <v>30</v>
       </c>
-      <c r="D31" s="37" t="s">
+      <c r="D31" s="24" t="s">
         <v>44</v>
       </c>
       <c r="E31" s="5"/>
@@ -1854,7 +1854,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="23" t="s">
         <v>41</v>
       </c>
       <c r="C32" s="5">
@@ -1870,7 +1870,7 @@
       </c>
     </row>
     <row r="33" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="23" t="s">
         <v>42</v>
       </c>
       <c r="C33" s="5">
@@ -1886,7 +1886,7 @@
       </c>
     </row>
     <row r="34" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="23" t="s">
         <v>43</v>
       </c>
       <c r="C34" s="5">
@@ -2071,17 +2071,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BM4">
     <cfRule type="expression" dxfId="8" priority="8">
@@ -2136,7 +2136,7 @@
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="47" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <headerFooter differentFirst="1">
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
filter feature fix and new feature
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billy\OneDrive\Desktop\Software Technologies\GitWorkspace\Project Management\2810ICT-Project-Management-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A03599-98DA-4C76-8E48-5CE89D857CB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{292C8F9C-99FD-4F2D-BA96-51E727FB3D4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -222,9 +222,6 @@
     <t>3.5 Implement Nutrition Level Filter Feature</t>
   </si>
   <si>
-    <t>3.6 Implement ADDITIONAL FEATURE</t>
-  </si>
-  <si>
     <t>3.7 Conduct Testing</t>
   </si>
   <si>
@@ -250,6 +247,9 @@
   </si>
   <si>
     <t>Ongoing</t>
+  </si>
+  <si>
+    <t>3.6 Implement Food Wars Feature</t>
   </si>
 </sst>
 </file>
@@ -635,6 +635,33 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -646,33 +673,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -1076,8 +1076,8 @@
   </sheetPr>
   <dimension ref="B1:BM40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BQ2" sqref="BQ2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1104,11 +1104,11 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:65" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1116,37 +1116,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="29"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="33"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="29"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="37"/>
+      <c r="V2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="35" t="s">
+      <c r="AA2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="33"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1160,22 +1160,22 @@
       <c r="AP2" s="20"/>
     </row>
     <row r="3" spans="2:65" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="25" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1202,12 +1202,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="27"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1759,7 +1759,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B26" s="23" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C26" s="5">
         <v>45</v>
@@ -1775,7 +1775,7 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C27" s="5">
         <v>50</v>
@@ -1791,13 +1791,13 @@
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C28" s="5">
         <v>1</v>
       </c>
       <c r="D28" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1807,13 +1807,13 @@
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="23" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" s="5">
         <v>30</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
@@ -1823,13 +1823,13 @@
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C30" s="5">
         <v>30</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
@@ -1839,13 +1839,13 @@
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B31" s="23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="5">
         <v>30</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B32" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C32" s="5">
         <v>55</v>
@@ -1871,7 +1871,7 @@
     </row>
     <row r="33" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B33" s="23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C33" s="5">
         <v>56</v>
@@ -1887,7 +1887,7 @@
     </row>
     <row r="34" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B34" s="23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="5">
         <v>57</v>
@@ -2071,17 +2071,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BM4">
     <cfRule type="expression" dxfId="8" priority="8">

</xml_diff>

<commit_message>
filling out actual start dates as I go
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billy\OneDrive\Desktop\Software Technologies\GitWorkspace\Project Management\2810ICT-Project-Management-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AB6F8C-4DA2-491E-96B6-ED1CAD9B7A0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4027E778-CD79-4EBF-8D59-0C0F2AE19731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -635,6 +635,33 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
       <alignment vertical="center"/>
     </xf>
@@ -646,33 +673,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -696,7 +696,818 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="66">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="7"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1074,10 +1885,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BM40"/>
+  <dimension ref="B1:BS40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="CC11" sqref="CC11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1093,7 +1904,7 @@
     <col min="42" max="42" width="2.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:65" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
+    <row r="1" spans="2:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
       <c r="B1" s="11" t="s">
         <v>13</v>
       </c>
@@ -1103,12 +1914,12 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:65" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="25"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
+    <row r="2" spans="2:71" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
       <c r="G2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1116,37 +1927,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="31" t="s">
+      <c r="K2" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="33"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="29"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="31" t="s">
+      <c r="Q2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="33"/>
+      <c r="R2" s="30"/>
+      <c r="S2" s="30"/>
+      <c r="T2" s="29"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="36"/>
-      <c r="X2" s="36"/>
-      <c r="Y2" s="37"/>
+      <c r="V2" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="33"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="35" t="s">
+      <c r="AA2" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="36"/>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="37"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="33"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1159,23 +1970,23 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:65" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="26" t="s">
+    <row r="3" spans="2:71" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="28" t="s">
+      <c r="D3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="28" t="s">
+      <c r="F3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="25" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1201,13 +2012,13 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="2:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="27"/>
-      <c r="C4" s="29"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
+    <row r="4" spans="2:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="36"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1382,8 +2193,26 @@
       <c r="BM4" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="BN4" s="3">
+        <v>59</v>
+      </c>
+      <c r="BO4" s="3">
+        <v>60</v>
+      </c>
+      <c r="BP4" s="3">
+        <v>61</v>
+      </c>
+      <c r="BQ4" s="3">
+        <v>62</v>
+      </c>
+      <c r="BR4" s="3">
+        <v>63</v>
+      </c>
+      <c r="BS4" s="3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="23" t="s">
         <v>14</v>
       </c>
@@ -1403,7 +2232,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="23" t="s">
         <v>15</v>
       </c>
@@ -1423,7 +2252,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="23" t="s">
         <v>16</v>
       </c>
@@ -1443,7 +2272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B8" s="23" t="s">
         <v>17</v>
       </c>
@@ -1463,7 +2292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
@@ -1483,7 +2312,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="23" t="s">
         <v>19</v>
       </c>
@@ -1503,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1523,7 +2352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="23" t="s">
         <v>21</v>
       </c>
@@ -1543,7 +2372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B13" s="23" t="s">
         <v>22</v>
       </c>
@@ -1563,7 +2392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B14" s="23" t="s">
         <v>23</v>
       </c>
@@ -1583,7 +2412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B15" s="23" t="s">
         <v>24</v>
       </c>
@@ -1603,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:65" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B16" s="23" t="s">
         <v>25</v>
       </c>
@@ -1729,7 +2558,9 @@
       <c r="D22" s="5">
         <v>3</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="5">
+        <v>46</v>
+      </c>
       <c r="F22" s="5"/>
       <c r="G22" s="22">
         <v>0</v>
@@ -2097,46 +2928,202 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:BM4">
-    <cfRule type="expression" dxfId="8" priority="8">
+  <conditionalFormatting sqref="H4:BS4">
+    <cfRule type="expression" dxfId="65" priority="56">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:BM34">
+    <cfRule type="expression" dxfId="64" priority="49">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="63" priority="51">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="62" priority="52">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="61" priority="53">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="60" priority="54">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="59" priority="55">
+      <formula>H$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="58" priority="59">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="57" priority="60">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BN5:BN34">
+    <cfRule type="expression" dxfId="47" priority="41">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="46" priority="42">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="45" priority="43">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="44" priority="44">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="43" priority="45">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="42" priority="46">
+      <formula>BN$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="41" priority="47">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="40" priority="48">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BO5:BO34">
+    <cfRule type="expression" dxfId="39" priority="33">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="38" priority="34">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="37" priority="35">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="36">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="35" priority="37">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="34" priority="38">
+      <formula>BO$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="33" priority="39">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="32" priority="40">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BP5:BP34">
+    <cfRule type="expression" dxfId="31" priority="25">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="30" priority="26">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="29" priority="27">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="28">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="29">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="26" priority="30">
+      <formula>BP$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="25" priority="31">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="24" priority="32">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BQ5:BQ34">
+    <cfRule type="expression" dxfId="23" priority="17">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="22" priority="18">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="21" priority="19">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="20" priority="20">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="19" priority="21">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="18" priority="22">
+      <formula>BQ$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="17" priority="23">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BR5:BR34">
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="11">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="12">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="13">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="10" priority="14">
+      <formula>BR$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="15">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="16">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BS5:BS34">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="3">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="4">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="7">
-      <formula>H$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="11">
+    <cfRule type="expression" dxfId="2" priority="6">
+      <formula>BS$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="12">
+    <cfRule type="expression" dxfId="0" priority="8">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
extended chart added more dates
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billy\OneDrive\Desktop\Software Technologies\GitWorkspace\Project Management\2810ICT-Project-Management-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4027E778-CD79-4EBF-8D59-0C0F2AE19731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67249A67-14FA-47FF-902D-C8B71D83AF02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -635,12 +635,24 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -661,18 +673,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -696,818 +696,7 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="66">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="9" tint="0.59996337778862885"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7"/>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor auto="1"/>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-      <border>
-        <bottom style="thin">
-          <color theme="0"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </left>
-        <right style="thin">
-          <color theme="9" tint="-0.24994659260841701"/>
-        </right>
-        <bottom style="thin">
-          <color theme="7"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <fill>
         <patternFill>
@@ -1887,8 +1076,8 @@
   </sheetPr>
   <dimension ref="B1:BS40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="CC11" sqref="CC11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1915,11 +1104,11 @@
       <c r="G1" s="10"/>
     </row>
     <row r="2" spans="2:71" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1927,37 +1116,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="29"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="29"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="33"/>
+      <c r="V2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="31" t="s">
+      <c r="AA2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="33"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="37"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1971,22 +1160,22 @@
       <c r="AP2" s="20"/>
     </row>
     <row r="3" spans="2:71" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="30" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -2013,12 +1202,12 @@
       <c r="AA3" s="8"/>
     </row>
     <row r="4" spans="2:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="36"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -2656,7 +1845,9 @@
       <c r="D28" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="5">
+        <v>46</v>
+      </c>
       <c r="F28" s="5"/>
       <c r="G28" s="22">
         <v>0</v>
@@ -2672,7 +1863,9 @@
       <c r="D29" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E29" s="5"/>
+      <c r="E29" s="5">
+        <v>46</v>
+      </c>
       <c r="F29" s="5"/>
       <c r="G29" s="22">
         <v>0</v>
@@ -2688,7 +1881,9 @@
       <c r="D30" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="5"/>
+      <c r="E30" s="5">
+        <v>46</v>
+      </c>
       <c r="F30" s="5"/>
       <c r="G30" s="22">
         <v>0</v>
@@ -2704,7 +1899,9 @@
       <c r="D31" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="5"/>
+      <c r="E31" s="5">
+        <v>46</v>
+      </c>
       <c r="F31" s="5"/>
       <c r="G31" s="22">
         <v>0</v>
@@ -2928,180 +2125,24 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
   <conditionalFormatting sqref="H4:BS4">
-    <cfRule type="expression" dxfId="65" priority="56">
+    <cfRule type="expression" dxfId="8" priority="56">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BM34">
-    <cfRule type="expression" dxfId="64" priority="49">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="63" priority="51">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="62" priority="52">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="61" priority="53">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="60" priority="54">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="59" priority="55">
-      <formula>H$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="58" priority="59">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="57" priority="60">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BN5:BN34">
-    <cfRule type="expression" dxfId="47" priority="41">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="46" priority="42">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="43">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="44">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="43" priority="45">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="42" priority="46">
-      <formula>BN$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="41" priority="47">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="40" priority="48">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BO5:BO34">
-    <cfRule type="expression" dxfId="39" priority="33">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="34">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="37" priority="35">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="36">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="35" priority="37">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="34" priority="38">
-      <formula>BO$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="33" priority="39">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="32" priority="40">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BP5:BP34">
-    <cfRule type="expression" dxfId="31" priority="25">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="30" priority="26">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="29" priority="27">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="28">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="27" priority="29">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="26" priority="30">
-      <formula>BP$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="25" priority="31">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BQ5:BQ34">
-    <cfRule type="expression" dxfId="23" priority="17">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="22" priority="18">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="21" priority="19">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="20" priority="20">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="19" priority="21">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="22">
-      <formula>BQ$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="23">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BR5:BR34">
-    <cfRule type="expression" dxfId="15" priority="9">
-      <formula>PercentComplete</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="14" priority="10">
-      <formula>PercentCompleteBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="13" priority="11">
-      <formula>Actual</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="12">
-      <formula>ActualBeyond</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>Plan</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14">
-      <formula>BR$4=period_selected</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15">
-      <formula>MOD(COLUMN(),2)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16">
-      <formula>MOD(COLUMN(),2)=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BS5:BS34">
+  <conditionalFormatting sqref="H5:BS34">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -3118,7 +2159,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="2" priority="6">
-      <formula>BS$4=period_selected</formula>
+      <formula>H$4=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="7">
       <formula>MOD(COLUMN(),2)</formula>

</xml_diff>

<commit_message>
Added specific testing to gantt chart
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billy\OneDrive\Desktop\Software Technologies\GitWorkspace\Project Management\2810ICT-Project-Management-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132CD657-73BD-40B8-BE94-28243CC20053}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC87590-AF61-410E-BCF3-F35833A6CDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="47">
   <si>
     <t>PERIODS</t>
   </si>
@@ -222,9 +222,6 @@
     <t>3.5 Implement Nutrition Level Filter Feature</t>
   </si>
   <si>
-    <t>3.7 Conduct Testing</t>
-  </si>
-  <si>
     <t>4.1 Track Progress</t>
   </si>
   <si>
@@ -250,6 +247,15 @@
   </si>
   <si>
     <t>3.6 Implement Food Wars Feature</t>
+  </si>
+  <si>
+    <t>3.7 Executive Summary</t>
+  </si>
+  <si>
+    <t>3.8 Unit Testing and Report</t>
+  </si>
+  <si>
+    <t>3.9 Coverage Testing and Report</t>
   </si>
 </sst>
 </file>
@@ -1074,10 +1080,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BS40"/>
+  <dimension ref="B1:BS42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E18" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="Z21" sqref="Z21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="S27" sqref="S27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1783,7 +1789,9 @@
       <c r="D24" s="5">
         <v>3</v>
       </c>
-      <c r="E24" s="5"/>
+      <c r="E24" s="5">
+        <v>50</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" s="22">
         <v>0</v>
@@ -1799,7 +1807,9 @@
       <c r="D25" s="5">
         <v>3</v>
       </c>
-      <c r="E25" s="5"/>
+      <c r="E25" s="5">
+        <v>50</v>
+      </c>
       <c r="F25" s="5"/>
       <c r="G25" s="22">
         <v>0</v>
@@ -1807,7 +1817,7 @@
     </row>
     <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B26" s="23" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" s="5">
         <v>45</v>
@@ -1823,65 +1833,55 @@
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B27" s="23" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C27" s="5">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D27" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
-      <c r="G27" s="22">
-        <v>0</v>
-      </c>
+      <c r="G27" s="22"/>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="23" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C28" s="5">
-        <v>1</v>
-      </c>
-      <c r="D28" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="5">
-        <v>46</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
+      </c>
+      <c r="E28" s="5"/>
       <c r="F28" s="5"/>
-      <c r="G28" s="22">
-        <v>0</v>
-      </c>
+      <c r="G28" s="22"/>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="23" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C29" s="5">
-        <v>30</v>
-      </c>
-      <c r="D29" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E29" s="5">
-        <v>46</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2</v>
+      </c>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="22">
-        <v>0</v>
-      </c>
+      <c r="G29" s="22"/>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="23" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C30" s="5">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="D30" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E30" s="5">
         <v>46</v>
@@ -1893,13 +1893,13 @@
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B31" s="23" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C31" s="5">
         <v>30</v>
       </c>
       <c r="D31" s="24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E31" s="5">
         <v>46</v>
@@ -1911,15 +1911,17 @@
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B32" s="23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C32" s="5">
-        <v>55</v>
-      </c>
-      <c r="D32" s="5">
-        <v>1</v>
-      </c>
-      <c r="E32" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E32" s="5">
+        <v>46</v>
+      </c>
       <c r="F32" s="5"/>
       <c r="G32" s="22">
         <v>0</v>
@@ -1927,15 +1929,17 @@
     </row>
     <row r="33" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B33" s="23" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C33" s="5">
-        <v>56</v>
-      </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5"/>
+        <v>30</v>
+      </c>
+      <c r="D33" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="5">
+        <v>46</v>
+      </c>
       <c r="F33" s="5"/>
       <c r="G33" s="22">
         <v>0</v>
@@ -1943,10 +1947,10 @@
     </row>
     <row r="34" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B34" s="23" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C34" s="5">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D34" s="5">
         <v>1</v>
@@ -1957,61 +1961,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B35"/>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
-      <c r="F35"/>
-      <c r="G35"/>
-      <c r="H35"/>
-      <c r="I35"/>
-      <c r="J35"/>
-      <c r="K35"/>
-      <c r="L35"/>
-      <c r="M35"/>
-      <c r="N35"/>
-      <c r="O35"/>
-      <c r="P35"/>
-      <c r="Q35"/>
-      <c r="R35"/>
-      <c r="S35"/>
-      <c r="T35"/>
-      <c r="U35"/>
-      <c r="V35"/>
-      <c r="W35"/>
-      <c r="X35"/>
-      <c r="Y35"/>
-      <c r="Z35"/>
-      <c r="AA35"/>
-    </row>
-    <row r="36" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B36"/>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
-      <c r="F36"/>
-      <c r="G36"/>
-      <c r="H36"/>
-      <c r="I36"/>
-      <c r="J36"/>
-      <c r="K36"/>
-      <c r="L36"/>
-      <c r="M36"/>
-      <c r="N36"/>
-      <c r="O36"/>
-      <c r="P36"/>
-      <c r="Q36"/>
-      <c r="R36"/>
-      <c r="S36"/>
-      <c r="T36"/>
-      <c r="U36"/>
-      <c r="V36"/>
-      <c r="W36"/>
-      <c r="X36"/>
-      <c r="Y36"/>
-      <c r="Z36"/>
-      <c r="AA36"/>
+    <row r="35" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B35" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="5">
+        <v>56</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="B36" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="5">
+        <v>57</v>
+      </c>
+      <c r="D36" s="5">
+        <v>1</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="22">
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B37"/>
@@ -2125,6 +2105,62 @@
       <c r="Z40"/>
       <c r="AA40"/>
     </row>
+    <row r="41" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+      <c r="Z41"/>
+      <c r="AA41"/>
+    </row>
+    <row r="42" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+      <c r="Z42"/>
+      <c r="AA42"/>
+    </row>
   </sheetData>
   <mergeCells count="11">
     <mergeCell ref="B2:F2"/>
@@ -2144,7 +2180,7 @@
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BS34">
+  <conditionalFormatting sqref="H5:BS36">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>

</xml_diff>

<commit_message>
Gantt chart completely finished
</commit_message>
<xml_diff>
--- a/Gantt chart.xlsx
+++ b/Gantt chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Billy\OneDrive\Desktop\Software Technologies\GitWorkspace\Project Management\2810ICT-Project-Management-Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEDD540-9405-40A8-AB6D-7BF3642FC3A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E509C664-96C5-4D76-9CB2-97E44C2E26E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="12196" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -641,12 +641,24 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="5" xfId="10" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="10" applyFont="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -667,18 +679,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="12">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="9" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="10" applyFont="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -702,7 +702,120 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="17">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1080,10 +1193,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BS42"/>
+  <dimension ref="B1:BQ42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="BF28" sqref="BF28"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="49" zoomScaleNormal="45" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="CB4" sqref="CB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.73046875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.5"/>
@@ -1099,7 +1212,7 @@
     <col min="42" max="42" width="2.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:71" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
+    <row r="1" spans="2:69" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.6">
       <c r="B1" s="11" t="s">
         <v>13</v>
       </c>
@@ -1109,12 +1222,12 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="2:71" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+    <row r="2" spans="2:69" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
       <c r="G2" s="21" t="s">
         <v>11</v>
       </c>
@@ -1122,37 +1235,37 @@
         <v>1</v>
       </c>
       <c r="J2" s="13"/>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="L2" s="28"/>
-      <c r="M2" s="28"/>
-      <c r="N2" s="28"/>
-      <c r="O2" s="29"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="33"/>
       <c r="P2" s="14"/>
-      <c r="Q2" s="27" t="s">
+      <c r="Q2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="29"/>
+      <c r="R2" s="34"/>
+      <c r="S2" s="34"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="15"/>
-      <c r="V2" s="31" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="33"/>
+      <c r="V2" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="36"/>
+      <c r="X2" s="36"/>
+      <c r="Y2" s="37"/>
       <c r="Z2" s="16"/>
-      <c r="AA2" s="31" t="s">
+      <c r="AA2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="33"/>
+      <c r="AB2" s="36"/>
+      <c r="AC2" s="36"/>
+      <c r="AD2" s="36"/>
+      <c r="AE2" s="36"/>
+      <c r="AF2" s="36"/>
+      <c r="AG2" s="37"/>
       <c r="AH2" s="17"/>
       <c r="AI2" s="19" t="s">
         <v>3</v>
@@ -1165,23 +1278,23 @@
       <c r="AO2" s="20"/>
       <c r="AP2" s="20"/>
     </row>
-    <row r="3" spans="2:71" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="35" t="s">
+    <row r="3" spans="2:69" s="9" customFormat="1" ht="39.950000000000003" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="37" t="s">
+      <c r="C3" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="37" t="s">
+      <c r="D3" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="37" t="s">
+      <c r="E3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="37" t="s">
+      <c r="F3" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="30" t="s">
         <v>10</v>
       </c>
       <c r="H3" s="18" t="s">
@@ -1207,13 +1320,13 @@
       <c r="Z3" s="8"/>
       <c r="AA3" s="8"/>
     </row>
-    <row r="4" spans="2:71" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="36"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
+    <row r="4" spans="2:69" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B4" s="27"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="3">
         <v>1</v>
       </c>
@@ -1400,14 +1513,8 @@
       <c r="BQ4" s="3">
         <v>62</v>
       </c>
-      <c r="BR4" s="3">
-        <v>63</v>
-      </c>
-      <c r="BS4" s="3">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    </row>
+    <row r="5" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B5" s="23" t="s">
         <v>14</v>
       </c>
@@ -1427,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="6" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B6" s="23" t="s">
         <v>15</v>
       </c>
@@ -1447,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="7" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B7" s="23" t="s">
         <v>16</v>
       </c>
@@ -1467,7 +1574,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B8" s="23" t="s">
         <v>17</v>
       </c>
@@ -1487,7 +1594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B9" s="23" t="s">
         <v>18</v>
       </c>
@@ -1507,7 +1614,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B10" s="23" t="s">
         <v>19</v>
       </c>
@@ -1527,7 +1634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B11" s="23" t="s">
         <v>20</v>
       </c>
@@ -1547,7 +1654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B12" s="23" t="s">
         <v>21</v>
       </c>
@@ -1567,7 +1674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B13" s="23" t="s">
         <v>22</v>
       </c>
@@ -1587,7 +1694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="14" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B14" s="23" t="s">
         <v>23</v>
       </c>
@@ -1607,7 +1714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B15" s="23" t="s">
         <v>24</v>
       </c>
@@ -1627,7 +1734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:71" ht="30" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:69" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B16" s="23" t="s">
         <v>25</v>
       </c>
@@ -1740,9 +1847,11 @@
       <c r="E21" s="5">
         <v>50</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="5">
+        <v>12</v>
+      </c>
       <c r="G21" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1778,9 +1887,11 @@
       <c r="E23" s="5">
         <v>46</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="5">
+        <v>15</v>
+      </c>
       <c r="G23" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1836,9 +1947,11 @@
       <c r="E26" s="5">
         <v>55</v>
       </c>
-      <c r="F26" s="5"/>
+      <c r="F26" s="5">
+        <v>6</v>
+      </c>
       <c r="G26" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1851,9 +1964,15 @@
       <c r="D27" s="5">
         <v>3</v>
       </c>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="22"/>
+      <c r="E27" s="5">
+        <v>61</v>
+      </c>
+      <c r="F27" s="5">
+        <v>1</v>
+      </c>
+      <c r="G27" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B28" s="23" t="s">
@@ -1868,8 +1987,12 @@
       <c r="E28" s="5">
         <v>53</v>
       </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="22"/>
+      <c r="F28" s="5">
+        <v>8</v>
+      </c>
+      <c r="G28" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B29" s="23" t="s">
@@ -1881,9 +2004,15 @@
       <c r="D29" s="5">
         <v>2</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="22"/>
+      <c r="E29" s="5">
+        <v>60</v>
+      </c>
+      <c r="F29" s="5">
+        <v>2</v>
+      </c>
+      <c r="G29" s="22">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B30" s="23" t="s">
@@ -1898,9 +2027,11 @@
       <c r="E30" s="5">
         <v>46</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="5">
+        <v>16</v>
+      </c>
       <c r="G30" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1916,9 +2047,11 @@
       <c r="E31" s="5">
         <v>46</v>
       </c>
-      <c r="F31" s="5"/>
+      <c r="F31" s="5">
+        <v>16</v>
+      </c>
       <c r="G31" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1934,9 +2067,11 @@
       <c r="E32" s="5">
         <v>46</v>
       </c>
-      <c r="F32" s="5"/>
+      <c r="F32" s="5">
+        <v>16</v>
+      </c>
       <c r="G32" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1952,9 +2087,11 @@
       <c r="E33" s="5">
         <v>46</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="5">
+        <v>16</v>
+      </c>
       <c r="G33" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1967,10 +2104,14 @@
       <c r="D34" s="5">
         <v>1</v>
       </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
+      <c r="E34" s="5">
+        <v>61</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
       <c r="G34" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1983,10 +2124,14 @@
       <c r="D35" s="5">
         <v>1</v>
       </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
+      <c r="E35" s="5">
+        <v>61</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
       <c r="G35" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.5">
@@ -1999,10 +2144,14 @@
       <c r="D36" s="5">
         <v>1</v>
       </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
+      <c r="E36" s="5">
+        <v>61</v>
+      </c>
+      <c r="F36" s="5">
+        <v>1</v>
+      </c>
       <c r="G36" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:27" ht="30" customHeight="1" x14ac:dyDescent="0.45">
@@ -2175,46 +2324,72 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="V2:Y2"/>
+    <mergeCell ref="AA2:AG2"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H4:BS4">
-    <cfRule type="expression" dxfId="8" priority="56">
+  <conditionalFormatting sqref="H4:BQ4">
+    <cfRule type="expression" dxfId="16" priority="56">
       <formula>H$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H5:BS36">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="H21:BB21 H25:BH25 BE21:BL21 BN21:BQ21 H22:BQ24 H26:BQ36 BK25:BQ25 H5:BQ20">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>PercentCompleteBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="13" priority="3">
       <formula>Actual</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="12" priority="4">
       <formula>ActualBeyond</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>Plan</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="10" priority="6">
       <formula>H$4=period_selected</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>MOD(COLUMN(),2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>MOD(COLUMN(),2)=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BD21 BM21 BJ25">
+    <cfRule type="expression" dxfId="7" priority="65">
+      <formula>PercentComplete</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="66">
+      <formula>PercentCompleteBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="67">
+      <formula>Actual</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="68">
+      <formula>ActualBeyond</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="69">
+      <formula>Plan</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="70">
+      <formula>BC$4=period_selected</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="71">
+      <formula>MOD(COLUMN(),2)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="72">
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>